<commit_message>
finished MVP and added Readme
</commit_message>
<xml_diff>
--- a/data/SandwichPrefsData.xlsx
+++ b/data/SandwichPrefsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\senio\Documents\Programming\Python Scripts\VSCode\AGE\Class\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF645CD8-304D-46AB-9B2F-9E98FE70554D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{15D5518E-3E7F-4C74-9126-FDC9DAB6D065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="16220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="73">
   <si>
     <t>ID</t>
   </si>
@@ -188,6 +188,63 @@
   </si>
   <si>
     <t>#6 The Boss;#8 The Great Garlic;#7 The Mexicali;</t>
+  </si>
+  <si>
+    <t>#17 Garlic Roast Beef;#2 The Outlaw;#11 Subway Club;</t>
+  </si>
+  <si>
+    <t>#99 Grand Slam Ham;#15 Titan Turkey;#20 Elite Chicken &amp; Bacon Ranch;</t>
+  </si>
+  <si>
+    <t>#1 The Philly;#6 The Boss;#19 Pickleball Club;</t>
+  </si>
+  <si>
+    <t>#33 Teriyaki Blitz;#16 All-Pro Sweet Onion Teriyaki;</t>
+  </si>
+  <si>
+    <t>#10 All-American Club;#11 Subway Club;#20 Elite Chicken &amp; Bacon Ranch;</t>
+  </si>
+  <si>
+    <t>#8 The Great Garlic;</t>
+  </si>
+  <si>
+    <t>#15 Titan Turkey;#7 The Mexicali;#9 The Champ;</t>
+  </si>
+  <si>
+    <t>#15 Titan Turkey;#33 Teriyaki Blitz;</t>
+  </si>
+  <si>
+    <t>Veggie Delight;</t>
+  </si>
+  <si>
+    <t>#1 The Philly;#20 Elite Chicken &amp; Bacon Ranch;#3 The Monster;</t>
+  </si>
+  <si>
+    <t>#23 The Hotshot Italiano;#20 Elite Chicken &amp; Bacon Ranch;</t>
+  </si>
+  <si>
+    <t>#11 Subway Club;</t>
+  </si>
+  <si>
+    <t>#1 The Philly;#33 Teriyaki Blitz;#6 The Boss;</t>
+  </si>
+  <si>
+    <t>#15 Titan Turkey;#33 Teriyaki Blitz;#20 Elite Chicken &amp; Bacon Ranch;</t>
+  </si>
+  <si>
+    <t>#15 Titan Turkey;#6 The Boss;#20 Elite Chicken &amp; Bacon Ranch;</t>
+  </si>
+  <si>
+    <t>#23 The Hotshot Italiano;#6 The Boss;#33 Teriyaki Blitz;</t>
+  </si>
+  <si>
+    <t>#33 Teriyaki Blitz;</t>
+  </si>
+  <si>
+    <t>#30 The Beast;#33 Teriyaki Blitz;#20 Elite Chicken &amp; Bacon Ranch;</t>
+  </si>
+  <si>
+    <t>#6 The Boss;#33 Teriyaki Blitz;</t>
   </si>
 </sst>
 </file>
@@ -275,8 +332,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:I45" totalsRowShown="0">
-  <autoFilter ref="A1:I45" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:I68" totalsRowShown="0">
+  <autoFilter ref="A1:I68" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="8"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Start time" dataDxfId="7"/>
@@ -589,17 +646,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I45"/>
+  <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="6" width="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="54.1796875" customWidth="1"/>
-    <col min="8" max="9" width="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="9" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
@@ -1685,6 +1740,558 @@
       </c>
       <c r="I45" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" s="1">
+        <v>45184.7866319444</v>
+      </c>
+      <c r="C46" s="1">
+        <v>45184.7874421296</v>
+      </c>
+      <c r="D46" t="s">
+        <v>9</v>
+      </c>
+      <c r="F46" s="1"/>
+      <c r="G46" t="s">
+        <v>54</v>
+      </c>
+      <c r="H46" t="s">
+        <v>11</v>
+      </c>
+      <c r="I46" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" s="1">
+        <v>45185.166828703703</v>
+      </c>
+      <c r="C47" s="1">
+        <v>45185.167905092603</v>
+      </c>
+      <c r="D47" t="s">
+        <v>9</v>
+      </c>
+      <c r="F47" s="1"/>
+      <c r="G47" t="s">
+        <v>55</v>
+      </c>
+      <c r="H47" t="s">
+        <v>14</v>
+      </c>
+      <c r="I47" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" s="1">
+        <v>45185.340833333299</v>
+      </c>
+      <c r="C48" s="1">
+        <v>45185.341238425899</v>
+      </c>
+      <c r="D48" t="s">
+        <v>9</v>
+      </c>
+      <c r="F48" s="1"/>
+      <c r="G48" t="s">
+        <v>56</v>
+      </c>
+      <c r="H48" t="s">
+        <v>21</v>
+      </c>
+      <c r="I48" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" s="1">
+        <v>45185.598946759303</v>
+      </c>
+      <c r="C49" s="1">
+        <v>45185.599247685197</v>
+      </c>
+      <c r="D49" t="s">
+        <v>9</v>
+      </c>
+      <c r="F49" s="1"/>
+      <c r="G49" t="s">
+        <v>57</v>
+      </c>
+      <c r="H49" t="s">
+        <v>11</v>
+      </c>
+      <c r="I49" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" s="1">
+        <v>45186.055277777799</v>
+      </c>
+      <c r="C50" s="1">
+        <v>45186.056064814802</v>
+      </c>
+      <c r="D50" t="s">
+        <v>9</v>
+      </c>
+      <c r="F50" s="1"/>
+      <c r="G50" t="s">
+        <v>58</v>
+      </c>
+      <c r="H50" t="s">
+        <v>11</v>
+      </c>
+      <c r="I50" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" s="1">
+        <v>45186.325266203698</v>
+      </c>
+      <c r="C51" s="1">
+        <v>45186.325937499998</v>
+      </c>
+      <c r="D51" t="s">
+        <v>9</v>
+      </c>
+      <c r="F51" s="1"/>
+      <c r="G51" t="s">
+        <v>59</v>
+      </c>
+      <c r="H51" t="s">
+        <v>11</v>
+      </c>
+      <c r="I51" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" s="1">
+        <v>45187.105717592603</v>
+      </c>
+      <c r="C52" s="1">
+        <v>45187.106145833299</v>
+      </c>
+      <c r="D52" t="s">
+        <v>9</v>
+      </c>
+      <c r="F52" s="1"/>
+      <c r="G52" t="s">
+        <v>60</v>
+      </c>
+      <c r="H52" t="s">
+        <v>14</v>
+      </c>
+      <c r="I52" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" s="1">
+        <v>45188.139965277798</v>
+      </c>
+      <c r="C53" s="1">
+        <v>45188.140138888899</v>
+      </c>
+      <c r="D53" t="s">
+        <v>9</v>
+      </c>
+      <c r="F53" s="1"/>
+      <c r="G53" t="s">
+        <v>61</v>
+      </c>
+      <c r="H53" t="s">
+        <v>14</v>
+      </c>
+      <c r="I53" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" s="1">
+        <v>45188.846168981501</v>
+      </c>
+      <c r="C54" s="1">
+        <v>45188.846458333297</v>
+      </c>
+      <c r="D54" t="s">
+        <v>9</v>
+      </c>
+      <c r="F54" s="1"/>
+      <c r="G54" t="s">
+        <v>25</v>
+      </c>
+      <c r="H54" t="s">
+        <v>14</v>
+      </c>
+      <c r="I54" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" s="1">
+        <v>45188.998865740701</v>
+      </c>
+      <c r="C55" s="1">
+        <v>45188.9990972222</v>
+      </c>
+      <c r="D55" t="s">
+        <v>9</v>
+      </c>
+      <c r="F55" s="1"/>
+      <c r="G55" t="s">
+        <v>62</v>
+      </c>
+      <c r="H55" t="s">
+        <v>11</v>
+      </c>
+      <c r="I55" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" s="1">
+        <v>45189.5770486111</v>
+      </c>
+      <c r="C56" s="1">
+        <v>45189.577465277798</v>
+      </c>
+      <c r="D56" t="s">
+        <v>9</v>
+      </c>
+      <c r="F56" s="1"/>
+      <c r="G56" t="s">
+        <v>63</v>
+      </c>
+      <c r="H56" t="s">
+        <v>11</v>
+      </c>
+      <c r="I56" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" s="1">
+        <v>45191.550300925897</v>
+      </c>
+      <c r="C57" s="1">
+        <v>45191.550787036998</v>
+      </c>
+      <c r="D57" t="s">
+        <v>9</v>
+      </c>
+      <c r="F57" s="1"/>
+      <c r="G57" t="s">
+        <v>64</v>
+      </c>
+      <c r="H57" t="s">
+        <v>21</v>
+      </c>
+      <c r="I57" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" s="1">
+        <v>45191.550821759301</v>
+      </c>
+      <c r="C58" s="1">
+        <v>45191.551076388903</v>
+      </c>
+      <c r="D58" t="s">
+        <v>9</v>
+      </c>
+      <c r="F58" s="1"/>
+      <c r="G58" t="s">
+        <v>65</v>
+      </c>
+      <c r="H58" t="s">
+        <v>21</v>
+      </c>
+      <c r="I58" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" s="1">
+        <v>45191.551111111097</v>
+      </c>
+      <c r="C59" s="1">
+        <v>45191.551238425898</v>
+      </c>
+      <c r="D59" t="s">
+        <v>9</v>
+      </c>
+      <c r="F59" s="1"/>
+      <c r="G59" t="s">
+        <v>62</v>
+      </c>
+      <c r="H59" t="s">
+        <v>21</v>
+      </c>
+      <c r="I59" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" s="1">
+        <v>45191.551284722198</v>
+      </c>
+      <c r="C60" s="1">
+        <v>45191.551863425899</v>
+      </c>
+      <c r="D60" t="s">
+        <v>9</v>
+      </c>
+      <c r="F60" s="1"/>
+      <c r="G60" t="s">
+        <v>66</v>
+      </c>
+      <c r="H60" t="s">
+        <v>11</v>
+      </c>
+      <c r="I60" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" s="1">
+        <v>45191.5518981481</v>
+      </c>
+      <c r="C61" s="1">
+        <v>45191.552129629599</v>
+      </c>
+      <c r="D61" t="s">
+        <v>9</v>
+      </c>
+      <c r="F61" s="1"/>
+      <c r="G61" t="s">
+        <v>67</v>
+      </c>
+      <c r="H61" t="s">
+        <v>11</v>
+      </c>
+      <c r="I61" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" s="1">
+        <v>45191.552152777796</v>
+      </c>
+      <c r="C62" s="1">
+        <v>45191.552326388897</v>
+      </c>
+      <c r="D62" t="s">
+        <v>9</v>
+      </c>
+      <c r="F62" s="1"/>
+      <c r="G62" t="s">
+        <v>68</v>
+      </c>
+      <c r="H62" t="s">
+        <v>11</v>
+      </c>
+      <c r="I62" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" s="1">
+        <v>45191.552349537</v>
+      </c>
+      <c r="C63" s="1">
+        <v>45191.5524421296</v>
+      </c>
+      <c r="D63" t="s">
+        <v>9</v>
+      </c>
+      <c r="F63" s="1"/>
+      <c r="G63" t="s">
+        <v>24</v>
+      </c>
+      <c r="H63" t="s">
+        <v>11</v>
+      </c>
+      <c r="I63" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" s="1">
+        <v>45191.552465277797</v>
+      </c>
+      <c r="C64" s="1">
+        <v>45191.552731481497</v>
+      </c>
+      <c r="D64" t="s">
+        <v>9</v>
+      </c>
+      <c r="F64" s="1"/>
+      <c r="G64" t="s">
+        <v>69</v>
+      </c>
+      <c r="H64" t="s">
+        <v>11</v>
+      </c>
+      <c r="I64" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" s="1">
+        <v>45191.552743055603</v>
+      </c>
+      <c r="C65" s="1">
+        <v>45191.552835648101</v>
+      </c>
+      <c r="D65" t="s">
+        <v>9</v>
+      </c>
+      <c r="F65" s="1"/>
+      <c r="G65" t="s">
+        <v>70</v>
+      </c>
+      <c r="H65" t="s">
+        <v>11</v>
+      </c>
+      <c r="I65" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66" s="1">
+        <v>45191.961064814801</v>
+      </c>
+      <c r="C66" s="1">
+        <v>45191.961550925902</v>
+      </c>
+      <c r="D66" t="s">
+        <v>9</v>
+      </c>
+      <c r="F66" s="1"/>
+      <c r="G66" t="s">
+        <v>71</v>
+      </c>
+      <c r="H66" t="s">
+        <v>21</v>
+      </c>
+      <c r="I66" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" s="1">
+        <v>45192.572581018503</v>
+      </c>
+      <c r="C67" s="1">
+        <v>45192.572812500002</v>
+      </c>
+      <c r="D67" t="s">
+        <v>9</v>
+      </c>
+      <c r="F67" s="1"/>
+      <c r="G67" t="s">
+        <v>62</v>
+      </c>
+      <c r="H67" t="s">
+        <v>14</v>
+      </c>
+      <c r="I67" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68" s="1">
+        <v>45195.453090277799</v>
+      </c>
+      <c r="C68" s="1">
+        <v>45195.453460648103</v>
+      </c>
+      <c r="D68" t="s">
+        <v>9</v>
+      </c>
+      <c r="F68" s="1"/>
+      <c r="G68" t="s">
+        <v>72</v>
+      </c>
+      <c r="H68" t="s">
+        <v>14</v>
+      </c>
+      <c r="I68" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bug fixes regarding terminal input and multiple camera uses
</commit_message>
<xml_diff>
--- a/data/SandwichPrefsData.xlsx
+++ b/data/SandwichPrefsData.xlsx
@@ -17,8 +17,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="166" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="166" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -78,7 +78,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -87,7 +87,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,7 +466,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E69"/>
+  <dimension ref="A1:E75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -499,7 +500,7 @@
       <c r="A2" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="n">
+      <c r="B2" s="5" t="n">
         <v>45183.63403935185</v>
       </c>
       <c r="C2" t="inlineStr">
@@ -522,7 +523,7 @@
       <c r="A3" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="n">
+      <c r="B3" s="5" t="n">
         <v>45183.64886574074</v>
       </c>
       <c r="C3" t="inlineStr">
@@ -545,7 +546,7 @@
       <c r="A4" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="n">
+      <c r="B4" s="5" t="n">
         <v>45183.68490740741</v>
       </c>
       <c r="C4" t="inlineStr">
@@ -568,7 +569,7 @@
       <c r="A5" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="4" t="n">
+      <c r="B5" s="5" t="n">
         <v>45183.69966435185</v>
       </c>
       <c r="C5" t="inlineStr">
@@ -591,7 +592,7 @@
       <c r="A6" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="4" t="n">
+      <c r="B6" s="5" t="n">
         <v>45183.70039351852</v>
       </c>
       <c r="C6" t="inlineStr">
@@ -614,7 +615,7 @@
       <c r="A7" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="4" t="n">
+      <c r="B7" s="5" t="n">
         <v>45183.7009837963</v>
       </c>
       <c r="C7" t="inlineStr">
@@ -637,7 +638,7 @@
       <c r="A8" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="4" t="n">
+      <c r="B8" s="5" t="n">
         <v>45183.70614583333</v>
       </c>
       <c r="C8" t="inlineStr">
@@ -660,7 +661,7 @@
       <c r="A9" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="B9" s="4" t="n">
+      <c r="B9" s="5" t="n">
         <v>45183.71555555556</v>
       </c>
       <c r="C9" t="inlineStr">
@@ -683,7 +684,7 @@
       <c r="A10" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="B10" s="4" t="n">
+      <c r="B10" s="5" t="n">
         <v>45183.72936342593</v>
       </c>
       <c r="C10" t="inlineStr">
@@ -706,7 +707,7 @@
       <c r="A11" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="B11" s="4" t="n">
+      <c r="B11" s="5" t="n">
         <v>45183.74293981482</v>
       </c>
       <c r="C11" t="inlineStr">
@@ -729,7 +730,7 @@
       <c r="A12" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="B12" s="4" t="n">
+      <c r="B12" s="5" t="n">
         <v>45183.746875</v>
       </c>
       <c r="C12" t="inlineStr">
@@ -752,7 +753,7 @@
       <c r="A13" s="3" t="n">
         <v>11</v>
       </c>
-      <c r="B13" s="4" t="n">
+      <c r="B13" s="5" t="n">
         <v>45183.75841435185</v>
       </c>
       <c r="C13" t="inlineStr">
@@ -775,7 +776,7 @@
       <c r="A14" s="3" t="n">
         <v>12</v>
       </c>
-      <c r="B14" s="4" t="n">
+      <c r="B14" s="5" t="n">
         <v>45183.76342592593</v>
       </c>
       <c r="C14" t="inlineStr">
@@ -798,7 +799,7 @@
       <c r="A15" s="3" t="n">
         <v>13</v>
       </c>
-      <c r="B15" s="4" t="n">
+      <c r="B15" s="5" t="n">
         <v>45183.76599537037</v>
       </c>
       <c r="C15" t="inlineStr">
@@ -821,7 +822,7 @@
       <c r="A16" s="3" t="n">
         <v>14</v>
       </c>
-      <c r="B16" s="4" t="n">
+      <c r="B16" s="5" t="n">
         <v>45183.76833333333</v>
       </c>
       <c r="C16" t="inlineStr">
@@ -844,7 +845,7 @@
       <c r="A17" s="3" t="n">
         <v>15</v>
       </c>
-      <c r="B17" s="4" t="n">
+      <c r="B17" s="5" t="n">
         <v>45183.76832175926</v>
       </c>
       <c r="C17" t="inlineStr">
@@ -867,7 +868,7 @@
       <c r="A18" s="3" t="n">
         <v>16</v>
       </c>
-      <c r="B18" s="4" t="n">
+      <c r="B18" s="5" t="n">
         <v>45183.7696412037</v>
       </c>
       <c r="C18" t="inlineStr">
@@ -890,7 +891,7 @@
       <c r="A19" s="3" t="n">
         <v>17</v>
       </c>
-      <c r="B19" s="4" t="n">
+      <c r="B19" s="5" t="n">
         <v>45183.77094907407</v>
       </c>
       <c r="C19" t="inlineStr">
@@ -913,7 +914,7 @@
       <c r="A20" s="3" t="n">
         <v>18</v>
       </c>
-      <c r="B20" s="4" t="n">
+      <c r="B20" s="5" t="n">
         <v>45183.7841087963</v>
       </c>
       <c r="C20" t="inlineStr">
@@ -936,7 +937,7 @@
       <c r="A21" s="3" t="n">
         <v>19</v>
       </c>
-      <c r="B21" s="4" t="n">
+      <c r="B21" s="5" t="n">
         <v>45183.78340277778</v>
       </c>
       <c r="C21" t="inlineStr">
@@ -959,7 +960,7 @@
       <c r="A22" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="B22" s="4" t="n">
+      <c r="B22" s="5" t="n">
         <v>45183.80048611111</v>
       </c>
       <c r="C22" t="inlineStr">
@@ -982,7 +983,7 @@
       <c r="A23" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="B23" s="4" t="n">
+      <c r="B23" s="5" t="n">
         <v>45183.80634259259</v>
       </c>
       <c r="C23" t="inlineStr">
@@ -1005,7 +1006,7 @@
       <c r="A24" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="B24" s="4" t="n">
+      <c r="B24" s="5" t="n">
         <v>45183.81844907408</v>
       </c>
       <c r="C24" t="inlineStr">
@@ -1028,7 +1029,7 @@
       <c r="A25" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="B25" s="4" t="n">
+      <c r="B25" s="5" t="n">
         <v>45183.85221064815</v>
       </c>
       <c r="C25" t="inlineStr">
@@ -1051,7 +1052,7 @@
       <c r="A26" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="B26" s="4" t="n">
+      <c r="B26" s="5" t="n">
         <v>45183.85377314815</v>
       </c>
       <c r="C26" t="inlineStr">
@@ -1074,7 +1075,7 @@
       <c r="A27" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="B27" s="4" t="n">
+      <c r="B27" s="5" t="n">
         <v>45183.85893518518</v>
       </c>
       <c r="C27" t="inlineStr">
@@ -1097,7 +1098,7 @@
       <c r="A28" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="B28" s="4" t="n">
+      <c r="B28" s="5" t="n">
         <v>45183.87486111111</v>
       </c>
       <c r="C28" t="inlineStr">
@@ -1120,7 +1121,7 @@
       <c r="A29" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="B29" s="4" t="n">
+      <c r="B29" s="5" t="n">
         <v>45183.91740740741</v>
       </c>
       <c r="C29" t="inlineStr">
@@ -1143,7 +1144,7 @@
       <c r="A30" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="B30" s="4" t="n">
+      <c r="B30" s="5" t="n">
         <v>45183.92065972222</v>
       </c>
       <c r="C30" t="inlineStr">
@@ -1166,7 +1167,7 @@
       <c r="A31" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="B31" s="4" t="n">
+      <c r="B31" s="5" t="n">
         <v>45183.94469907408</v>
       </c>
       <c r="C31" t="inlineStr">
@@ -1189,7 +1190,7 @@
       <c r="A32" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="B32" s="4" t="n">
+      <c r="B32" s="5" t="n">
         <v>45183.9584375</v>
       </c>
       <c r="C32" t="inlineStr">
@@ -1212,7 +1213,7 @@
       <c r="A33" s="3" t="n">
         <v>31</v>
       </c>
-      <c r="B33" s="4" t="n">
+      <c r="B33" s="5" t="n">
         <v>45183.95909722222</v>
       </c>
       <c r="C33" t="inlineStr">
@@ -1235,7 +1236,7 @@
       <c r="A34" s="3" t="n">
         <v>32</v>
       </c>
-      <c r="B34" s="4" t="n">
+      <c r="B34" s="5" t="n">
         <v>45183.95987268518</v>
       </c>
       <c r="C34" t="inlineStr">
@@ -1258,7 +1259,7 @@
       <c r="A35" s="3" t="n">
         <v>33</v>
       </c>
-      <c r="B35" s="4" t="n">
+      <c r="B35" s="5" t="n">
         <v>45184.05405092592</v>
       </c>
       <c r="C35" t="inlineStr">
@@ -1281,7 +1282,7 @@
       <c r="A36" s="3" t="n">
         <v>34</v>
       </c>
-      <c r="B36" s="4" t="n">
+      <c r="B36" s="5" t="n">
         <v>45184.06104166667</v>
       </c>
       <c r="C36" t="inlineStr">
@@ -1304,7 +1305,7 @@
       <c r="A37" s="3" t="n">
         <v>35</v>
       </c>
-      <c r="B37" s="4" t="n">
+      <c r="B37" s="5" t="n">
         <v>45184.06890046296</v>
       </c>
       <c r="C37" t="inlineStr">
@@ -1327,7 +1328,7 @@
       <c r="A38" s="3" t="n">
         <v>36</v>
       </c>
-      <c r="B38" s="4" t="n">
+      <c r="B38" s="5" t="n">
         <v>45184.09741898148</v>
       </c>
       <c r="C38" t="inlineStr">
@@ -1350,7 +1351,7 @@
       <c r="A39" s="3" t="n">
         <v>37</v>
       </c>
-      <c r="B39" s="4" t="n">
+      <c r="B39" s="5" t="n">
         <v>45184.11915509259</v>
       </c>
       <c r="C39" t="inlineStr">
@@ -1373,7 +1374,7 @@
       <c r="A40" s="3" t="n">
         <v>38</v>
       </c>
-      <c r="B40" s="4" t="n">
+      <c r="B40" s="5" t="n">
         <v>45184.23310185185</v>
       </c>
       <c r="C40" t="inlineStr">
@@ -1396,7 +1397,7 @@
       <c r="A41" s="3" t="n">
         <v>39</v>
       </c>
-      <c r="B41" s="4" t="n">
+      <c r="B41" s="5" t="n">
         <v>45184.35518518519</v>
       </c>
       <c r="C41" t="inlineStr">
@@ -1419,7 +1420,7 @@
       <c r="A42" s="3" t="n">
         <v>40</v>
       </c>
-      <c r="B42" s="4" t="n">
+      <c r="B42" s="5" t="n">
         <v>45184.40028935186</v>
       </c>
       <c r="C42" t="inlineStr">
@@ -1442,7 +1443,7 @@
       <c r="A43" s="3" t="n">
         <v>41</v>
       </c>
-      <c r="B43" s="4" t="n">
+      <c r="B43" s="5" t="n">
         <v>45184.50071759259</v>
       </c>
       <c r="C43" t="inlineStr">
@@ -1465,7 +1466,7 @@
       <c r="A44" s="3" t="n">
         <v>42</v>
       </c>
-      <c r="B44" s="4" t="n">
+      <c r="B44" s="5" t="n">
         <v>45184.51079861111</v>
       </c>
       <c r="C44" t="inlineStr">
@@ -1488,7 +1489,7 @@
       <c r="A45" s="3" t="n">
         <v>43</v>
       </c>
-      <c r="B45" s="4" t="n">
+      <c r="B45" s="5" t="n">
         <v>45184.6362037037</v>
       </c>
       <c r="C45" t="inlineStr">
@@ -1511,7 +1512,7 @@
       <c r="A46" s="3" t="n">
         <v>44</v>
       </c>
-      <c r="B46" s="4" t="n">
+      <c r="B46" s="5" t="n">
         <v>45184.78663194444</v>
       </c>
       <c r="C46" t="inlineStr">
@@ -1534,7 +1535,7 @@
       <c r="A47" s="3" t="n">
         <v>45</v>
       </c>
-      <c r="B47" s="4" t="n">
+      <c r="B47" s="5" t="n">
         <v>45185.1668287037</v>
       </c>
       <c r="C47" t="inlineStr">
@@ -1557,7 +1558,7 @@
       <c r="A48" s="3" t="n">
         <v>46</v>
       </c>
-      <c r="B48" s="4" t="n">
+      <c r="B48" s="5" t="n">
         <v>45185.34083333334</v>
       </c>
       <c r="C48" t="inlineStr">
@@ -1580,7 +1581,7 @@
       <c r="A49" s="3" t="n">
         <v>47</v>
       </c>
-      <c r="B49" s="4" t="n">
+      <c r="B49" s="5" t="n">
         <v>45185.59894675926</v>
       </c>
       <c r="C49" t="inlineStr">
@@ -1603,7 +1604,7 @@
       <c r="A50" s="3" t="n">
         <v>48</v>
       </c>
-      <c r="B50" s="4" t="n">
+      <c r="B50" s="5" t="n">
         <v>45186.05527777778</v>
       </c>
       <c r="C50" t="inlineStr">
@@ -1626,7 +1627,7 @@
       <c r="A51" s="3" t="n">
         <v>49</v>
       </c>
-      <c r="B51" s="4" t="n">
+      <c r="B51" s="5" t="n">
         <v>45186.3252662037</v>
       </c>
       <c r="C51" t="inlineStr">
@@ -1649,7 +1650,7 @@
       <c r="A52" s="3" t="n">
         <v>50</v>
       </c>
-      <c r="B52" s="4" t="n">
+      <c r="B52" s="5" t="n">
         <v>45187.1057175926</v>
       </c>
       <c r="C52" t="inlineStr">
@@ -1672,7 +1673,7 @@
       <c r="A53" s="3" t="n">
         <v>51</v>
       </c>
-      <c r="B53" s="4" t="n">
+      <c r="B53" s="5" t="n">
         <v>45188.13996527778</v>
       </c>
       <c r="C53" t="inlineStr">
@@ -1695,7 +1696,7 @@
       <c r="A54" s="3" t="n">
         <v>52</v>
       </c>
-      <c r="B54" s="4" t="n">
+      <c r="B54" s="5" t="n">
         <v>45188.84616898148</v>
       </c>
       <c r="C54" t="inlineStr">
@@ -1718,7 +1719,7 @@
       <c r="A55" s="3" t="n">
         <v>53</v>
       </c>
-      <c r="B55" s="4" t="n">
+      <c r="B55" s="5" t="n">
         <v>45188.99886574074</v>
       </c>
       <c r="C55" t="inlineStr">
@@ -1741,7 +1742,7 @@
       <c r="A56" s="3" t="n">
         <v>54</v>
       </c>
-      <c r="B56" s="4" t="n">
+      <c r="B56" s="5" t="n">
         <v>45189.57704861111</v>
       </c>
       <c r="C56" t="inlineStr">
@@ -1764,7 +1765,7 @@
       <c r="A57" s="3" t="n">
         <v>55</v>
       </c>
-      <c r="B57" s="4" t="n">
+      <c r="B57" s="5" t="n">
         <v>45191.55030092593</v>
       </c>
       <c r="C57" t="inlineStr">
@@ -1787,7 +1788,7 @@
       <c r="A58" s="3" t="n">
         <v>56</v>
       </c>
-      <c r="B58" s="4" t="n">
+      <c r="B58" s="5" t="n">
         <v>45191.55082175926</v>
       </c>
       <c r="C58" t="inlineStr">
@@ -1810,7 +1811,7 @@
       <c r="A59" s="3" t="n">
         <v>57</v>
       </c>
-      <c r="B59" s="4" t="n">
+      <c r="B59" s="5" t="n">
         <v>45191.55111111111</v>
       </c>
       <c r="C59" t="inlineStr">
@@ -1833,7 +1834,7 @@
       <c r="A60" s="3" t="n">
         <v>58</v>
       </c>
-      <c r="B60" s="4" t="n">
+      <c r="B60" s="5" t="n">
         <v>45191.55128472222</v>
       </c>
       <c r="C60" t="inlineStr">
@@ -1856,7 +1857,7 @@
       <c r="A61" s="3" t="n">
         <v>59</v>
       </c>
-      <c r="B61" s="4" t="n">
+      <c r="B61" s="5" t="n">
         <v>45191.55189814815</v>
       </c>
       <c r="C61" t="inlineStr">
@@ -1879,7 +1880,7 @@
       <c r="A62" s="3" t="n">
         <v>60</v>
       </c>
-      <c r="B62" s="4" t="n">
+      <c r="B62" s="5" t="n">
         <v>45191.55215277777</v>
       </c>
       <c r="C62" t="inlineStr">
@@ -1902,7 +1903,7 @@
       <c r="A63" s="3" t="n">
         <v>61</v>
       </c>
-      <c r="B63" s="4" t="n">
+      <c r="B63" s="5" t="n">
         <v>45191.55234953704</v>
       </c>
       <c r="C63" t="inlineStr">
@@ -1925,7 +1926,7 @@
       <c r="A64" s="3" t="n">
         <v>62</v>
       </c>
-      <c r="B64" s="4" t="n">
+      <c r="B64" s="5" t="n">
         <v>45191.55246527777</v>
       </c>
       <c r="C64" t="inlineStr">
@@ -1948,7 +1949,7 @@
       <c r="A65" s="3" t="n">
         <v>63</v>
       </c>
-      <c r="B65" s="4" t="n">
+      <c r="B65" s="5" t="n">
         <v>45191.55274305555</v>
       </c>
       <c r="C65" t="inlineStr">
@@ -1971,7 +1972,7 @@
       <c r="A66" s="3" t="n">
         <v>64</v>
       </c>
-      <c r="B66" s="4" t="n">
+      <c r="B66" s="5" t="n">
         <v>45191.96106481482</v>
       </c>
       <c r="C66" t="inlineStr">
@@ -1994,7 +1995,7 @@
       <c r="A67" s="3" t="n">
         <v>65</v>
       </c>
-      <c r="B67" s="4" t="n">
+      <c r="B67" s="5" t="n">
         <v>45192.57258101852</v>
       </c>
       <c r="C67" t="inlineStr">
@@ -2017,7 +2018,7 @@
       <c r="A68" s="3" t="n">
         <v>66</v>
       </c>
-      <c r="B68" s="4" t="n">
+      <c r="B68" s="5" t="n">
         <v>45195.45309027778</v>
       </c>
       <c r="C68" t="inlineStr">
@@ -2038,24 +2039,174 @@
     </row>
     <row r="69">
       <c r="A69" s="3" t="n">
+        <v>67</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>10/02/2023 18:00:33</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>25 - 32</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>#6 The Boss;</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="3" t="n">
+        <v>68</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>10/03/2023 13:19:11</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>60 - 100</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>#20 Elite Chicken &amp; Bacon Ranch;</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="3" t="n">
+        <v>69</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>10/04/2023 10:32:38</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>25 - 32</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>#4 Supreme Meats;</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="3" t="n">
+        <v>70</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>10/05/2023 13:26:56</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>15 - 20</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>#6 The Boss;</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="3" t="n">
+        <v>71</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>10/05/2023 13:28:37</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>60 - 100</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>#23 The Hotshot Italiano;</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="3" t="n">
+        <v>72</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>10/05/2023 13:30:06</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>60 - 100</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>#6 The Boss;</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="3" t="n">
         <v>-1</v>
       </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>10/02/2023 18:00:33</t>
-        </is>
-      </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>25 - 32</t>
-        </is>
-      </c>
-      <c r="D69" t="inlineStr">
-        <is>
-          <t>Male</t>
-        </is>
-      </c>
-      <c r="E69" t="inlineStr">
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>10/05/2023 13:30:34</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>0 - 2</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
         <is>
           <t>#6 The Boss;</t>
         </is>

</xml_diff>